<commit_message>
Atualizado por script em 31-10-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/india_isl_2023-2024.xlsx
+++ b/2023/india_isl_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2941,6 +2941,98 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>india</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>isl</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>45230.64583333334</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Odisha FC</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Bengaluru FC</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>27/10/2023 16:42</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>31/10/2023 15:29</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>27/10/2023 16:42</t>
+        </is>
+      </c>
+      <c r="P28" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>31/10/2023 15:29</t>
+        </is>
+      </c>
+      <c r="R28" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>27/10/2023 16:42</t>
+        </is>
+      </c>
+      <c r="T28" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>31/10/2023 15:29</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/india/isl/odisha-fc-bengaluru-fc/zsF6G8gj/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 01-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/india_isl_2023-2024.xlsx
+++ b/2023/india_isl_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3033,6 +3033,98 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>india</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>isl</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>45231.64583333334</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Jamshedpur</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>2</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Mohun Bagan</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>3</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>31/10/2023 15:30</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>01/11/2023 15:29</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>31/10/2023 15:30</t>
+        </is>
+      </c>
+      <c r="P29" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>01/11/2023 15:29</t>
+        </is>
+      </c>
+      <c r="R29" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>31/10/2023 15:30</t>
+        </is>
+      </c>
+      <c r="T29" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>01/11/2023 15:29</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/india/isl/jamshedpur-mohun-bagan/EXDAFS8d/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 02-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/india_isl_2023-2024.xlsx
+++ b/2023/india_isl_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3125,6 +3125,98 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>india</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>isl</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>45232.64583333334</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Mumbai City</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>01/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L30" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>02/11/2023 15:02</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>01/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P30" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>02/11/2023 15:02</t>
+        </is>
+      </c>
+      <c r="R30" t="n">
+        <v>8.56</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>01/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T30" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>02/11/2023 15:02</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/india/isl/mumbai-city-minerva-punjab/GxhgvCoc/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 30-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/india_isl_2023-2024.xlsx
+++ b/2023/india_isl_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4137,6 +4137,98 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>india</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>isl</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>45260.64583333334</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Bengaluru FC</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>3</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>3</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>28/11/2023 15:42</t>
+        </is>
+      </c>
+      <c r="L41" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>30/11/2023 15:29</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>28/11/2023 15:42</t>
+        </is>
+      </c>
+      <c r="P41" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>30/11/2023 15:29</t>
+        </is>
+      </c>
+      <c r="R41" t="n">
+        <v>5.24</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>28/11/2023 15:42</t>
+        </is>
+      </c>
+      <c r="T41" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>30/11/2023 15:29</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/india/isl/bengaluru-fc-minerva-punjab/GdKvj9p9/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>